<commit_message>
cross-section and panel results from IMSS data
</commit_message>
<xml_diff>
--- a/Tables/did_ind_imss.xlsx
+++ b/Tables/did_ind_imss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Statistics\P27\IMSS\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FDEAA97-BD7D-4C16-BBBC-851183A5FC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D722C25-743C-4ED8-A419-F1D4CA7CFF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B99C67BC-3728-455A-9901-4F0951BF3394}"/>
+    <workbookView xWindow="30660" yWindow="1860" windowWidth="21600" windowHeight="11175" xr2:uid="{B99C67BC-3728-455A-9901-4F0951BF3394}"/>
   </bookViews>
   <sheets>
     <sheet name="did_ind_imss" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Observations</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Four years after</t>
+  </si>
+  <si>
+    <t>(= 1)</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,6 +180,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -211,122 +217,167 @@
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>0.033</v>
+            <v>0.0062***</v>
           </cell>
           <cell r="C5" t="str">
-            <v>0.029</v>
+            <v>0.0098***</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>-0.0017</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6" t="str">
-            <v>(0.022)</v>
+            <v>(0.0011)</v>
           </cell>
           <cell r="C6" t="str">
-            <v>(0.022)</v>
+            <v>(0.0011)</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>(0.0082)</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8" t="str">
-            <v>0.022</v>
+            <v>0.0047***</v>
           </cell>
           <cell r="C8" t="str">
-            <v>0.020</v>
+            <v>0.0069***</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>-0.00024</v>
           </cell>
         </row>
         <row r="9">
           <cell r="B9" t="str">
-            <v>(0.015)</v>
+            <v>(0.00077)</v>
           </cell>
           <cell r="C9" t="str">
-            <v>(0.015)</v>
+            <v>(0.00077)</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>(0.0055)</v>
           </cell>
         </row>
         <row r="11">
           <cell r="B11" t="str">
-            <v>0.0078</v>
+            <v>0.0019***</v>
           </cell>
           <cell r="C11" t="str">
-            <v>0.0071</v>
+            <v>0.0031***</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>-0.0025</v>
           </cell>
         </row>
         <row r="12">
           <cell r="B12" t="str">
-            <v>(0.0086)</v>
+            <v>(0.00044)</v>
           </cell>
           <cell r="C12" t="str">
-            <v>(0.0085)</v>
+            <v>(0.00044)</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>(0.0031)</v>
           </cell>
         </row>
         <row r="14">
           <cell r="B14" t="str">
-            <v>-0.0051</v>
+            <v>-0.00091**</v>
           </cell>
           <cell r="C14" t="str">
-            <v>-0.0049</v>
+            <v>-0.0022***</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>0.0011</v>
           </cell>
         </row>
         <row r="15">
           <cell r="B15" t="str">
-            <v>(0.0085)</v>
+            <v>(0.00042)</v>
           </cell>
           <cell r="C15" t="str">
-            <v>(0.0085)</v>
+            <v>(0.00042)</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>(0.0029)</v>
           </cell>
         </row>
         <row r="17">
           <cell r="B17" t="str">
-            <v>-0.0042</v>
+            <v>-0.0013*</v>
           </cell>
           <cell r="C17" t="str">
-            <v>-0.0027</v>
+            <v>-0.0040***</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>-0.0012</v>
           </cell>
         </row>
         <row r="18">
           <cell r="B18" t="str">
-            <v>(0.014)</v>
+            <v>(0.00070)</v>
           </cell>
           <cell r="C18" t="str">
-            <v>(0.014)</v>
+            <v>(0.00069)</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v>(0.0047)</v>
           </cell>
         </row>
         <row r="20">
           <cell r="B20" t="str">
-            <v>-0.020</v>
+            <v>0.0011</v>
           </cell>
           <cell r="C20" t="str">
-            <v>-0.017</v>
+            <v>-0.0029***</v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>-0.0049</v>
           </cell>
         </row>
         <row r="21">
           <cell r="B21" t="str">
-            <v>(0.019)</v>
+            <v>(0.00094)</v>
           </cell>
           <cell r="C21" t="str">
-            <v>(0.018)</v>
+            <v>(0.00092)</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v>(0.0063)</v>
           </cell>
         </row>
         <row r="23">
           <cell r="B23" t="str">
-            <v>-0.019</v>
+            <v>0.0046***</v>
           </cell>
           <cell r="C23" t="str">
-            <v>-0.014</v>
+            <v>-0.00049</v>
+          </cell>
+          <cell r="D23" t="str">
+            <v>-0.0062</v>
           </cell>
         </row>
         <row r="24">
           <cell r="B24" t="str">
-            <v>(0.023)</v>
+            <v>(0.0011)</v>
           </cell>
           <cell r="C24" t="str">
-            <v>(0.022)</v>
+            <v>(0.0011)</v>
+          </cell>
+          <cell r="D24" t="str">
+            <v>(0.0075)</v>
           </cell>
         </row>
         <row r="26">
           <cell r="B26" t="str">
-            <v>-0.029</v>
+            <v>0.0093***</v>
           </cell>
           <cell r="C26" t="str">
-            <v>-0.021</v>
+            <v>0.0020</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>-0.011</v>
           </cell>
         </row>
         <row r="27">
@@ -334,18 +385,24 @@
             <v/>
           </cell>
           <cell r="B27" t="str">
-            <v>(0.027)</v>
+            <v>(0.0014)</v>
           </cell>
           <cell r="C27" t="str">
-            <v>(0.025)</v>
+            <v>(0.0013)</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>(0.0086)</v>
           </cell>
         </row>
         <row r="29">
           <cell r="B29" t="str">
-            <v>122433</v>
+            <v>49405618</v>
           </cell>
           <cell r="C29" t="str">
-            <v>121820</v>
+            <v>49229277</v>
+          </cell>
+          <cell r="D29" t="str">
+            <v>1051931</v>
           </cell>
         </row>
         <row r="30">
@@ -353,10 +410,13 @@
             <v>R-sq</v>
           </cell>
           <cell r="B30" t="str">
-            <v>0.123</v>
+            <v>0.125</v>
           </cell>
           <cell r="C30" t="str">
             <v>0.125</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v>0.244</v>
           </cell>
         </row>
         <row r="31">
@@ -364,18 +424,24 @@
             <v>DepVarMean</v>
           </cell>
           <cell r="B31" t="str">
-            <v>0.41</v>
+            <v>0.43</v>
           </cell>
           <cell r="C31" t="str">
-            <v>0.41</v>
+            <v>0.43</v>
+          </cell>
+          <cell r="D31" t="str">
+            <v>0.55</v>
           </cell>
         </row>
         <row r="32">
           <cell r="B32" t="str">
-            <v>531</v>
+            <v/>
           </cell>
           <cell r="C32" t="str">
-            <v>529</v>
+            <v/>
+          </cell>
+          <cell r="D32" t="str">
+            <v/>
           </cell>
         </row>
       </sheetData>
@@ -681,35 +747,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2F7EF6-16D9-44D3-ABCA-D1BD1BFACC09}">
-  <dimension ref="A2:C27"/>
+  <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D26" sqref="A2:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="10"/>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
         <f>[1]did_ind_imss!A2</f>
         <v/>
@@ -720,250 +792,339 @@
       <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>[1]did_ind_imss!B5</f>
-        <v>0.033</v>
+        <v>0.0062***</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>[1]did_ind_imss!C5</f>
-        <v>0.029</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.0098***</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>[1]did_ind_imss!D5</f>
+        <v>-0.0017</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="str">
         <f>[1]did_ind_imss!B6</f>
-        <v>(0.022)</v>
+        <v>(0.0011)</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>[1]did_ind_imss!C6</f>
-        <v>(0.022)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.0011)</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>[1]did_ind_imss!D6</f>
+        <v>(0.0082)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>[1]did_ind_imss!B8</f>
-        <v>0.022</v>
+        <v>0.0047***</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>[1]did_ind_imss!C8</f>
-        <v>0.020</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.0069***</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>[1]did_ind_imss!D8</f>
+        <v>-0.00024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="str">
         <f>[1]did_ind_imss!B9</f>
-        <v>(0.015)</v>
+        <v>(0.00077)</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>[1]did_ind_imss!C9</f>
-        <v>(0.015)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.00077)</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>[1]did_ind_imss!D9</f>
+        <v>(0.0055)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>[1]did_ind_imss!B11</f>
-        <v>0.0078</v>
+        <v>0.0019***</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>[1]did_ind_imss!C11</f>
-        <v>0.0071</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.0031***</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>[1]did_ind_imss!D11</f>
+        <v>-0.0025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="str">
         <f>[1]did_ind_imss!B12</f>
-        <v>(0.0086)</v>
+        <v>(0.00044)</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>[1]did_ind_imss!C12</f>
-        <v>(0.0085)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.00044)</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>[1]did_ind_imss!D12</f>
+        <v>(0.0031)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>[1]did_ind_imss!B14</f>
-        <v>-0.0051</v>
+        <v>-0.00091**</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>[1]did_ind_imss!C14</f>
-        <v>-0.0049</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-0.0022***</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>[1]did_ind_imss!D14</f>
+        <v>0.0011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="str">
         <f>[1]did_ind_imss!B15</f>
-        <v>(0.0085)</v>
+        <v>(0.00042)</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>[1]did_ind_imss!C15</f>
-        <v>(0.0085)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.00042)</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>[1]did_ind_imss!D15</f>
+        <v>(0.0029)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>[1]did_ind_imss!B17</f>
-        <v>-0.0042</v>
+        <v>-0.0013*</v>
       </c>
       <c r="C14" s="1" t="str">
         <f>[1]did_ind_imss!C17</f>
-        <v>-0.0027</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-0.0040***</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>[1]did_ind_imss!D17</f>
+        <v>-0.0012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="str">
         <f>[1]did_ind_imss!B18</f>
-        <v>(0.014)</v>
+        <v>(0.00070)</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>[1]did_ind_imss!C18</f>
-        <v>(0.014)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.00069)</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>[1]did_ind_imss!D18</f>
+        <v>(0.0047)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>[1]did_ind_imss!B20</f>
-        <v>-0.020</v>
+        <v>0.0011</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>[1]did_ind_imss!C20</f>
-        <v>-0.017</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-0.0029***</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>[1]did_ind_imss!D20</f>
+        <v>-0.0049</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="str">
         <f>[1]did_ind_imss!B21</f>
-        <v>(0.019)</v>
+        <v>(0.00094)</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>[1]did_ind_imss!C21</f>
-        <v>(0.018)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.00092)</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>[1]did_ind_imss!D21</f>
+        <v>(0.0063)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>[1]did_ind_imss!B23</f>
-        <v>-0.019</v>
+        <v>0.0046***</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>[1]did_ind_imss!C23</f>
-        <v>-0.014</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>-0.00049</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>[1]did_ind_imss!D23</f>
+        <v>-0.0062</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="str">
         <f>[1]did_ind_imss!B24</f>
-        <v>(0.023)</v>
+        <v>(0.0011)</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>[1]did_ind_imss!C24</f>
-        <v>(0.022)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.0011)</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f>[1]did_ind_imss!D24</f>
+        <v>(0.0075)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>[1]did_ind_imss!B26</f>
-        <v>-0.029</v>
+        <v>0.0093***</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>[1]did_ind_imss!C26</f>
-        <v>-0.021</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.0020</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>[1]did_ind_imss!D26</f>
+        <v>-0.011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>[1]did_ind_imss!A27</f>
         <v/>
       </c>
       <c r="B21" s="1" t="str">
         <f>[1]did_ind_imss!B27</f>
-        <v>(0.027)</v>
+        <v>(0.0014)</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>[1]did_ind_imss!C27</f>
-        <v>(0.025)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>(0.0013)</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f>[1]did_ind_imss!D27</f>
+        <v>(0.0086)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="9" t="str">
         <f>[1]did_ind_imss!B29</f>
-        <v>122433</v>
+        <v>49405618</v>
       </c>
       <c r="C23" s="9" t="str">
         <f>[1]did_ind_imss!C29</f>
-        <v>121820</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>49229277</v>
+      </c>
+      <c r="D23" s="9" t="str">
+        <f>[1]did_ind_imss!D29</f>
+        <v>1051931</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="str">
         <f>[1]did_ind_imss!B32</f>
-        <v>531</v>
+        <v/>
       </c>
       <c r="C24" s="1" t="str">
         <f>[1]did_ind_imss!C32</f>
-        <v>529</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v/>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f>[1]did_ind_imss!D32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>[1]did_ind_imss!A30</f>
         <v>R-sq</v>
       </c>
       <c r="B25" s="1" t="str">
         <f>[1]did_ind_imss!B30</f>
-        <v>0.123</v>
+        <v>0.125</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>[1]did_ind_imss!C30</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="1" t="str">
+        <f>[1]did_ind_imss!D30</f>
+        <v>0.244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="str">
         <f>[1]did_ind_imss!A31</f>
         <v>DepVarMean</v>
       </c>
       <c r="B26" s="7" t="str">
         <f>[1]did_ind_imss!B31</f>
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
       <c r="C26" s="7" t="str">
         <f>[1]did_ind_imss!C31</f>
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>0.43</v>
+      </c>
+      <c r="D26" s="7" t="str">
+        <f>[1]did_ind_imss!D31</f>
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>

</xml_diff>